<commit_message>
updated excel file and added logisim simulator
</commit_message>
<xml_diff>
--- a/Control.xlsx
+++ b/Control.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cambrown/dev/single_cycle_proc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96637B2-AF2F-C842-B1B5-C204D47D6254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4528B190-1BCB-3943-BE35-CF1E8E640122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9780" yWindow="1920" windowWidth="19940" windowHeight="17440" xr2:uid="{D642E7AC-0ECA-7B45-8310-35DFC7E3371B}"/>
   </bookViews>
@@ -502,7 +502,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -642,10 +642,10 @@
         <v>1</v>
       </c>
       <c r="H6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -668,10 +668,10 @@
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -694,7 +694,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="1">
         <v>1</v>

</xml_diff>